<commit_message>
operator counter initializer for cpp (partially final)
</commit_message>
<xml_diff>
--- a/smartcodelab-datasets/PythonCodes.xlsx
+++ b/smartcodelab-datasets/PythonCodes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magno\OneDrive\Desktop\Capstone 2\2025-CP_SMARTCODELAB\smartcodelab-datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Capstone 2\2025-CP_SMARTCODELAB\smartcodelab-datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C7D784-D035-438D-A7AB-F76A656445D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7F2B2B-D618-45DA-8E10-E1FBCC2D67BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1044,18 +1044,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="82.5703125" customWidth="1"/>
-    <col min="2" max="2" width="114.85546875" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" customWidth="1"/>
+    <col min="1" max="1" width="82.5546875" customWidth="1"/>
+    <col min="2" max="2" width="114.88671875" customWidth="1"/>
+    <col min="3" max="3" width="43.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="315" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="315" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="360" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="390" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="330" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="315" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="345" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="315" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="345" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="330" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="330" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="360" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="330" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>

</xml_diff>